<commit_message>
excel times for q2
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryd\OneDrive\Υπολογιστής\DBMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novap\OneDrive\Desktop\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F705A92-3DB6-477B-91AF-D689B7DA7AD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53492B8B-68A8-46F9-8191-89C5A26EB337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Ερώτημα</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>5A</t>
+  </si>
+  <si>
+    <t>0.631</t>
+  </si>
+  <si>
+    <t>0.643</t>
+  </si>
+  <si>
+    <t>0.700</t>
   </si>
 </sst>
 </file>
@@ -149,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -184,9 +193,16 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,7 +483,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3:E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,34 +623,52 @@
       <c r="B9" s="4">
         <v>1</v>
       </c>
+      <c r="D9" s="15">
+        <v>7.1749999999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="4">
         <v>2</v>
       </c>
+      <c r="D10" s="16">
+        <v>5.6000000000000001E-2</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D11" s="16">
+        <v>0.65400000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A12" s="5"/>
       <c r="B12" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="D12" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A13" s="5"/>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="D13" s="14" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B14" s="10" t="s">
         <v>6</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
this is not fun
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryd\OneDrive\Υπολογιστής\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D4B93F-0B2B-4D0F-9F94-FDE1D832EFD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A53E575-04B3-4214-9C80-2583DAD10424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -169,25 +169,22 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -473,7 +470,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:E14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +516,7 @@
       <c r="C3" s="12">
         <v>11.077999999999999</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="13">
         <v>7.3330000000000002</v>
       </c>
       <c r="E3">
@@ -532,7 +529,7 @@
       <c r="B4" s="4">
         <v>2</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="12">
         <v>0.10100000000000001</v>
       </c>
       <c r="D4" s="13">
@@ -592,7 +589,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="12">
@@ -629,10 +626,10 @@
       <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="11">
         <v>0.113</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="11">
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="E10">
@@ -645,10 +642,10 @@
       <c r="B11" s="4">
         <v>3</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="11">
         <v>1.119</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="11">
         <v>0.65400000000000003</v>
       </c>
       <c r="E11">
@@ -661,10 +658,10 @@
       <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="11">
         <v>1.03</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="10">
         <v>0.63100000000000001</v>
       </c>
       <c r="E12">
@@ -677,10 +674,10 @@
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="11">
         <v>1.0589999999999999</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13" s="10">
         <v>0.64300000000000002</v>
       </c>
       <c r="E13">
@@ -689,13 +686,13 @@
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="11">
         <v>1.119</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="10">
         <v>0.7</v>
       </c>
       <c r="E14">
@@ -736,7 +733,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>6</v>
       </c>
     </row>
@@ -773,7 +770,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add excel times q3
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryd\OneDrive\Υπολογιστής\DBMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novap\OneDrive\Desktop\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A53E575-04B3-4214-9C80-2583DAD10424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F3D552-2332-4353-A79A-52FC8D6C0478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -178,18 +178,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -207,7 +205,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Violet II">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -215,34 +213,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="632E62"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EAE5EB"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="92278F"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="9B57D3"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="755DD9"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="665EB8"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="45A5ED"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="5982DB"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0066FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="666699"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -470,7 +468,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -516,7 +514,7 @@
       <c r="C3" s="12">
         <v>11.077999999999999</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="10">
         <v>7.3330000000000002</v>
       </c>
       <c r="E3">
@@ -532,7 +530,7 @@
       <c r="C4" s="12">
         <v>0.10100000000000001</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="10">
         <v>0.06</v>
       </c>
       <c r="E4">
@@ -548,7 +546,7 @@
       <c r="C5" s="12">
         <v>1.0960000000000001</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="10">
         <v>0.61299999999999999</v>
       </c>
       <c r="E5">
@@ -564,7 +562,7 @@
       <c r="C6" s="12">
         <v>1.038</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="10">
         <v>0.59499999999999997</v>
       </c>
       <c r="E6">
@@ -580,7 +578,7 @@
       <c r="C7" s="12">
         <v>1.1160000000000001</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="10">
         <v>0.61299999999999999</v>
       </c>
       <c r="E7">
@@ -595,7 +593,7 @@
       <c r="C8" s="12">
         <v>1.2010000000000001</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="10">
         <v>0.64</v>
       </c>
       <c r="E8">
@@ -613,7 +611,7 @@
       <c r="C9" s="12">
         <v>9.5340000000000007</v>
       </c>
-      <c r="D9" s="14">
+      <c r="D9" s="11">
         <v>7.1749999999999998</v>
       </c>
       <c r="E9">
@@ -700,113 +698,159 @@
         <v>0.90949999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
         <v>3</v>
       </c>
       <c r="B15" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="C15" s="13"/>
+      <c r="D15" s="14">
+        <v>6.1859999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A16" s="5"/>
       <c r="B16" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C16" s="13"/>
+      <c r="D16" s="10">
+        <v>5.5E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
       <c r="B17" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C17" s="13"/>
+      <c r="D17" s="10">
+        <v>0.56899999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C18" s="13"/>
+      <c r="D18" s="10">
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C19" s="13"/>
+      <c r="D19" s="10">
+        <v>0.55700000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B20" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C20" s="13"/>
+      <c r="D20" s="10">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>4</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+    </row>
+    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C22" s="13"/>
+      <c r="D22" s="13"/>
+    </row>
+    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+    </row>
+    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+    </row>
+    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+    </row>
+    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>5</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+    </row>
+    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="4">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C28" s="13"/>
+      <c r="D28" s="13"/>
+    </row>
+    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C29" s="13"/>
+      <c r="D29" s="13"/>
+    </row>
+    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="4">
         <v>4</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="C30" s="13"/>
+      <c r="D30" s="13"/>
+    </row>
+    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C31" s="13"/>
+      <c r="D31" s="13"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
mary is da best
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novap\OneDrive\Desktop\DBMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maryd\OneDrive\Υπολογιστής\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30F3D552-2332-4353-A79A-52FC8D6C0478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC2CDAA-B003-437C-B279-F409FFD49AB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -149,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -181,13 +181,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Κανονικό" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14:E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,7 +533,7 @@
         <v>0.06</v>
       </c>
       <c r="E4">
-        <f t="shared" ref="E4:E14" si="0">(C4+D4)/2</f>
+        <f t="shared" ref="E4:E20" si="0">(C4+D4)/2</f>
         <v>8.0500000000000002E-2</v>
       </c>
     </row>
@@ -705,9 +704,15 @@
       <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14">
+      <c r="C15" s="13">
+        <v>6.6420000000000003</v>
+      </c>
+      <c r="D15" s="10">
         <v>6.1859999999999999</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>6.4139999999999997</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
@@ -715,142 +720,150 @@
       <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="13"/>
+      <c r="C16" s="13">
+        <v>0.111</v>
+      </c>
       <c r="D16" s="10">
         <v>5.5E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>8.3000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A17" s="5"/>
       <c r="B17" s="4">
         <v>3</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="13">
+        <v>1.0069999999999999</v>
+      </c>
       <c r="D17" s="10">
         <v>0.56899999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>0.78799999999999992</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A18" s="5"/>
       <c r="B18" s="4">
         <v>4</v>
       </c>
-      <c r="C18" s="13"/>
+      <c r="C18" s="13">
+        <v>1.095</v>
+      </c>
       <c r="D18" s="10">
         <v>0.60399999999999998</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="18.600000000000001" x14ac:dyDescent="0.4">
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>0.84949999999999992</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A19" s="5"/>
       <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="13"/>
+      <c r="C19" s="13">
+        <v>0.97799999999999998</v>
+      </c>
       <c r="D19" s="10">
         <v>0.55700000000000005</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
+      <c r="E19">
+        <f t="shared" si="0"/>
+        <v>0.76750000000000007</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B20" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="13"/>
+      <c r="C20" s="13">
+        <v>1.022</v>
+      </c>
       <c r="D20" s="10">
         <v>0.56000000000000005</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+      <c r="E20">
+        <f t="shared" si="0"/>
+        <v>0.79100000000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>4</v>
       </c>
       <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="13"/>
-    </row>
-    <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="22" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A22" s="5"/>
       <c r="B22" s="4">
         <v>2</v>
       </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="23" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="5"/>
       <c r="B23" s="4">
         <v>3</v>
       </c>
-      <c r="C23" s="13"/>
-      <c r="D23" s="13"/>
-    </row>
-    <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="24" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="5"/>
       <c r="B24" s="4">
         <v>4</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
-    </row>
-    <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="5"/>
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-    </row>
-    <row r="26" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B26" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-    </row>
-    <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="27" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="5">
         <v>5</v>
       </c>
       <c r="B27" s="4">
         <v>1</v>
       </c>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-    </row>
-    <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="6"/>
       <c r="B28" s="4">
         <v>2</v>
       </c>
-      <c r="C28" s="13"/>
-      <c r="D28" s="13"/>
-    </row>
-    <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="4">
         <v>3</v>
       </c>
-      <c r="C29" s="13"/>
-      <c r="D29" s="13"/>
-    </row>
-    <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="30" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="4">
         <v>4</v>
       </c>
-      <c r="C30" s="13"/>
-      <c r="D30" s="13"/>
-    </row>
-    <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="31" spans="1:5" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="13"/>
-      <c r="D31" s="13"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
added Ερώτημα 5 times :) <3 + epic python fail
</commit_message>
<xml_diff>
--- a/Times.xlsx
+++ b/Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\novap\OneDrive\Desktop\DBMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D410F5-FD4F-4534-94CD-76B81FF88447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{466F98CD-547B-43B6-BA8E-F64D76361FA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4860" yWindow="660" windowWidth="17496" windowHeight="12240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
   <si>
     <t>Ερώτημα</t>
   </si>
@@ -176,11 +176,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -518,11 +520,11 @@
       <c r="D3" s="10">
         <v>7.3330000000000002</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3">
         <f>(C3+D3)/2</f>
         <v>9.2055000000000007</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -537,11 +539,11 @@
       <c r="D4" s="10">
         <v>0.06</v>
       </c>
-      <c r="E4" s="11">
-        <f t="shared" ref="E4:E26" si="0">(C4+D4)/2</f>
+      <c r="E4">
+        <f t="shared" ref="E4:E32" si="0">(C4+D4)/2</f>
         <v>8.0500000000000002E-2</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -556,11 +558,11 @@
       <c r="D5" s="10">
         <v>0.61299999999999999</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5">
         <f t="shared" si="0"/>
         <v>0.85450000000000004</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -575,11 +577,11 @@
       <c r="D6" s="10">
         <v>0.59499999999999997</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6">
         <f t="shared" si="0"/>
         <v>0.8165</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -594,11 +596,11 @@
       <c r="D7" s="10">
         <v>0.61299999999999999</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7">
         <f t="shared" si="0"/>
         <v>0.86450000000000005</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -612,11 +614,11 @@
       <c r="D8" s="10">
         <v>0.64</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8">
         <f t="shared" si="0"/>
         <v>0.9205000000000001</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="13" t="s">
         <v>8</v>
       </c>
     </row>
@@ -630,14 +632,14 @@
       <c r="C9" s="10">
         <v>9.5340000000000007</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>7.1749999999999998</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9">
         <f t="shared" si="0"/>
         <v>8.3544999999999998</v>
       </c>
-      <c r="F9" s="13">
+      <c r="F9" s="12">
         <f>((E9 - E3)/E3)</f>
         <v>-9.2444734126337608E-2</v>
       </c>
@@ -647,18 +649,18 @@
       <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10" s="11">
         <v>0.113</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="11">
         <v>5.6000000000000001E-2</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>8.4500000000000006E-2</v>
       </c>
-      <c r="F10" s="13">
-        <f t="shared" ref="F10:F26" si="1">((E10 - E4)/E4)</f>
+      <c r="F10" s="12">
+        <f t="shared" ref="F10:F32" si="1">((E10 - E4)/E4)</f>
         <v>4.9689440993788865E-2</v>
       </c>
     </row>
@@ -667,17 +669,17 @@
       <c r="B11" s="4">
         <v>3</v>
       </c>
-      <c r="C11" s="12">
+      <c r="C11" s="11">
         <v>1.119</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="11">
         <v>0.65400000000000003</v>
       </c>
-      <c r="E11" s="11">
+      <c r="E11">
         <f t="shared" si="0"/>
         <v>0.88650000000000007</v>
       </c>
-      <c r="F11" s="13">
+      <c r="F11" s="12">
         <f t="shared" si="1"/>
         <v>3.7448800468110034E-2</v>
       </c>
@@ -687,17 +689,17 @@
       <c r="B12" s="4">
         <v>4</v>
       </c>
-      <c r="C12" s="12">
+      <c r="C12" s="11">
         <v>1.03</v>
       </c>
       <c r="D12" s="10">
         <v>0.63100000000000001</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>0.83050000000000002</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <f t="shared" si="1"/>
         <v>1.7146356399265171E-2</v>
       </c>
@@ -707,17 +709,17 @@
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="11">
         <v>1.0589999999999999</v>
       </c>
       <c r="D13" s="10">
         <v>0.64300000000000002</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>0.85099999999999998</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F13" s="12">
         <f t="shared" si="1"/>
         <v>-1.5615962984384115E-2</v>
       </c>
@@ -726,17 +728,17 @@
       <c r="B14" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="12">
+      <c r="C14" s="11">
         <v>1.119</v>
       </c>
       <c r="D14" s="10">
         <v>0.7</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14">
         <f t="shared" si="0"/>
         <v>0.90949999999999998</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F14" s="12">
         <f t="shared" si="1"/>
         <v>-1.1950027159152764E-2</v>
       </c>
@@ -748,17 +750,17 @@
       <c r="B15" s="4">
         <v>1</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="11">
         <v>6.6420000000000003</v>
       </c>
       <c r="D15" s="10">
         <v>6.1859999999999999</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15">
         <f t="shared" si="0"/>
         <v>6.4139999999999997</v>
       </c>
-      <c r="F15" s="13">
+      <c r="F15" s="12">
         <f t="shared" si="1"/>
         <v>-0.23227003411335209</v>
       </c>
@@ -768,17 +770,17 @@
       <c r="B16" s="4">
         <v>2</v>
       </c>
-      <c r="C16" s="12">
+      <c r="C16" s="11">
         <v>0.111</v>
       </c>
       <c r="D16" s="10">
         <v>5.5E-2</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16">
         <f t="shared" si="0"/>
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F16" s="13">
+      <c r="F16" s="12">
         <f t="shared" si="1"/>
         <v>-1.7751479289940843E-2</v>
       </c>
@@ -788,17 +790,17 @@
       <c r="B17" s="4">
         <v>3</v>
       </c>
-      <c r="C17" s="12">
+      <c r="C17" s="11">
         <v>1.0069999999999999</v>
       </c>
       <c r="D17" s="10">
         <v>0.56899999999999995</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17">
         <f t="shared" si="0"/>
         <v>0.78799999999999992</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="12">
         <f t="shared" si="1"/>
         <v>-0.11111111111111126</v>
       </c>
@@ -808,17 +810,17 @@
       <c r="B18" s="4">
         <v>4</v>
       </c>
-      <c r="C18" s="12">
+      <c r="C18" s="11">
         <v>1.095</v>
       </c>
       <c r="D18" s="10">
         <v>0.60399999999999998</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18">
         <f t="shared" si="0"/>
         <v>0.84949999999999992</v>
       </c>
-      <c r="F18" s="13">
+      <c r="F18" s="12">
         <f t="shared" si="1"/>
         <v>2.2877784467188328E-2</v>
       </c>
@@ -828,17 +830,17 @@
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="12">
+      <c r="C19" s="11">
         <v>0.97799999999999998</v>
       </c>
       <c r="D19" s="10">
         <v>0.55700000000000005</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19">
         <f t="shared" si="0"/>
         <v>0.76750000000000007</v>
       </c>
-      <c r="F19" s="13">
+      <c r="F19" s="12">
         <f t="shared" si="1"/>
         <v>-9.8119858989424102E-2</v>
       </c>
@@ -847,17 +849,17 @@
       <c r="B20" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="11">
         <v>1.022</v>
       </c>
       <c r="D20" s="10">
         <v>0.56000000000000005</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20">
         <f t="shared" si="0"/>
         <v>0.79100000000000004</v>
       </c>
-      <c r="F20" s="13">
+      <c r="F20" s="12">
         <f t="shared" si="1"/>
         <v>-0.13029136888400214</v>
       </c>
@@ -869,17 +871,17 @@
       <c r="B21" s="4">
         <v>1</v>
       </c>
-      <c r="C21" s="12">
+      <c r="C21" s="11">
         <v>8.1340000000000003</v>
       </c>
       <c r="D21" s="10">
         <v>5.7560000000000002</v>
       </c>
-      <c r="E21" s="11">
+      <c r="E21">
         <f>(C21+D21)/2</f>
         <v>6.9450000000000003</v>
       </c>
-      <c r="F21" s="13">
+      <c r="F21" s="12">
         <f t="shared" si="1"/>
         <v>8.2787652011225538E-2</v>
       </c>
@@ -889,17 +891,17 @@
       <c r="B22" s="4">
         <v>2</v>
       </c>
-      <c r="C22" s="12">
+      <c r="C22" s="11">
         <v>0.14699999999999999</v>
       </c>
       <c r="D22" s="10">
         <v>6.8000000000000005E-2</v>
       </c>
-      <c r="E22" s="11">
+      <c r="E22">
         <f t="shared" si="0"/>
         <v>0.1075</v>
       </c>
-      <c r="F22" s="13">
+      <c r="F22" s="12">
         <f t="shared" si="1"/>
         <v>0.29518072289156616</v>
       </c>
@@ -909,17 +911,17 @@
       <c r="B23" s="4">
         <v>3</v>
       </c>
-      <c r="C23" s="12">
+      <c r="C23" s="11">
         <v>0.317</v>
       </c>
       <c r="D23" s="10">
         <v>0.23799999999999999</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23">
         <f t="shared" si="0"/>
         <v>0.27749999999999997</v>
       </c>
-      <c r="F23" s="13">
+      <c r="F23" s="12">
         <f t="shared" si="1"/>
         <v>-0.64784263959390864</v>
       </c>
@@ -929,17 +931,17 @@
       <c r="B24" s="4">
         <v>4</v>
       </c>
-      <c r="C24" s="12">
+      <c r="C24" s="11">
         <v>0.436</v>
       </c>
       <c r="D24" s="10">
         <v>0.39</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24">
         <f t="shared" si="0"/>
         <v>0.41300000000000003</v>
       </c>
-      <c r="F24" s="13">
+      <c r="F24" s="12">
         <f t="shared" si="1"/>
         <v>-0.51383166568569738</v>
       </c>
@@ -949,17 +951,17 @@
       <c r="B25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="12">
+      <c r="C25" s="11">
         <v>0.32500000000000001</v>
       </c>
       <c r="D25" s="10">
         <v>0.22800000000000001</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25">
         <f t="shared" si="0"/>
         <v>0.27650000000000002</v>
       </c>
-      <c r="F25" s="13">
+      <c r="F25" s="12">
         <f t="shared" si="1"/>
         <v>-0.6397394136807818</v>
       </c>
@@ -968,17 +970,17 @@
       <c r="B26" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>0.47499999999999998</v>
       </c>
       <c r="D26" s="10">
         <v>0.39</v>
       </c>
-      <c r="E26" s="11">
+      <c r="E26">
         <f t="shared" si="0"/>
         <v>0.4325</v>
       </c>
-      <c r="F26" s="13">
+      <c r="F26" s="12">
         <f t="shared" si="1"/>
         <v>-0.45322376738305947</v>
       </c>
@@ -989,6 +991,18 @@
       </c>
       <c r="B27" s="4">
         <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.35">
@@ -996,28 +1010,96 @@
       <c r="B28" s="4">
         <v>2</v>
       </c>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="6"/>
       <c r="B29" s="4">
         <v>3</v>
       </c>
+      <c r="C29" s="11">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="E29">
+        <f t="shared" si="0"/>
+        <v>0.23049999999999998</v>
+      </c>
+      <c r="F29" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.16936936936936933</v>
+      </c>
     </row>
     <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="6"/>
       <c r="B30" s="4">
         <v>4</v>
       </c>
+      <c r="C30" s="11">
+        <v>0.312</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="E30">
+        <f t="shared" si="0"/>
+        <v>0.28900000000000003</v>
+      </c>
+      <c r="F30" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.3002421307506053</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="18" x14ac:dyDescent="0.35">
       <c r="A31" s="6"/>
       <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
+      <c r="C31" s="11">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="E31">
+        <f t="shared" si="0"/>
+        <v>0.21250000000000002</v>
+      </c>
+      <c r="F31" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.23146473779385171</v>
+      </c>
     </row>
     <row r="32" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B32" s="4" t="s">
         <v>5</v>
+      </c>
+      <c r="C32" s="11">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="0"/>
+        <v>0.3125</v>
+      </c>
+      <c r="F32" s="12">
+        <f t="shared" si="1"/>
+        <v>-0.2774566473988439</v>
       </c>
     </row>
   </sheetData>

</xml_diff>